<commit_message>
Replaced solder tip phone connector with three-pin MTA100
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="108">
   <si>
     <t>RefDes</t>
   </si>
@@ -322,6 +322,27 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/switchcraft-inc/RA49C14B/SC1541-ND/1289209</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Neutrik/NP3TT-P-R/?qs=sGAEpiMZZMvlX3nhDDO4ADUfAUIJI3vk17qNd8zaPfU%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Neutrik/NC3MXX-BAG/?qs=sGAEpiMZZMv0W4pxf2HiVxwZWAc2WDw0SRp5UVw1szU%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Neutrik/NC3FD-LX-HA-BAG/?qs=sGAEpiMZZMv0W4pxf2HiV9FjHoe8lE%252bzh2neYdjq12U%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Neutrik/BXX-2-RED/?qs=%2fha2pyFaduh9bwlS2wJrYXf3Cx2jUt5OYrvSBPEHSYg%3d</t>
+  </si>
+  <si>
+    <t>Neutrik XLR</t>
+  </si>
+  <si>
+    <t>640456-3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-3/A19470-ND/259010</t>
   </si>
 </sst>
 </file>
@@ -846,9 +867,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -867,6 +885,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1224,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,625 +1263,666 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="3" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="3" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="3" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="3" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="3" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="3" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="6">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="6">
+        <v>1</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="6">
+        <v>1</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H49" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H52" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H53" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H54" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="L58" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7">
+      <c r="M58" s="6">
         <v>1</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="N58" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
+      <c r="O58" s="6"/>
+      <c r="P58" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="3" t="s">
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="2" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="7">
-        <v>3</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="7">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="7">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="7">
-        <v>9</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="7">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="7">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="7">
-        <v>2</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="7">
-        <v>1</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="7">
-        <v>1</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="7">
-        <v>1</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="7">
-        <v>1</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="7">
-        <v>1</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H41" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H42" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H45" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="A26:B27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>
@@ -1869,31 +1931,37 @@
     <hyperlink ref="H7" r:id="rId4"/>
     <hyperlink ref="H8" r:id="rId5"/>
     <hyperlink ref="H9" r:id="rId6"/>
-    <hyperlink ref="H10" r:id="rId7"/>
+    <hyperlink ref="S58" r:id="rId7"/>
     <hyperlink ref="H11" r:id="rId8"/>
-    <hyperlink ref="H12" r:id="rId9"/>
-    <hyperlink ref="H13" r:id="rId10"/>
-    <hyperlink ref="H14" r:id="rId11"/>
-    <hyperlink ref="H15" r:id="rId12"/>
-    <hyperlink ref="H16" r:id="rId13"/>
-    <hyperlink ref="H17" r:id="rId14"/>
-    <hyperlink ref="H18" r:id="rId15"/>
-    <hyperlink ref="H19" r:id="rId16"/>
-    <hyperlink ref="H20" r:id="rId17"/>
-    <hyperlink ref="H21" r:id="rId18"/>
-    <hyperlink ref="H22" r:id="rId19"/>
+    <hyperlink ref="H13" r:id="rId9"/>
+    <hyperlink ref="H14" r:id="rId10"/>
+    <hyperlink ref="H15" r:id="rId11"/>
+    <hyperlink ref="H16" r:id="rId12"/>
+    <hyperlink ref="H17" r:id="rId13"/>
+    <hyperlink ref="H18" r:id="rId14"/>
+    <hyperlink ref="H19" r:id="rId15"/>
+    <hyperlink ref="H20" r:id="rId16"/>
+    <hyperlink ref="H21" r:id="rId17"/>
+    <hyperlink ref="H22" r:id="rId18"/>
+    <hyperlink ref="H23" r:id="rId19"/>
     <hyperlink ref="H6" r:id="rId20"/>
-    <hyperlink ref="H29" r:id="rId21"/>
-    <hyperlink ref="H30" r:id="rId22"/>
-    <hyperlink ref="H31" r:id="rId23"/>
-    <hyperlink ref="H32" r:id="rId24"/>
-    <hyperlink ref="H28" r:id="rId25"/>
-    <hyperlink ref="H38" r:id="rId26"/>
-    <hyperlink ref="H39" r:id="rId27"/>
-    <hyperlink ref="H42" r:id="rId28"/>
-    <hyperlink ref="H45" r:id="rId29"/>
+    <hyperlink ref="H30" r:id="rId21"/>
+    <hyperlink ref="H31" r:id="rId22"/>
+    <hyperlink ref="H32" r:id="rId23"/>
+    <hyperlink ref="H33" r:id="rId24"/>
+    <hyperlink ref="H29" r:id="rId25"/>
+    <hyperlink ref="H39" r:id="rId26"/>
+    <hyperlink ref="H40" r:id="rId27"/>
+    <hyperlink ref="H43" r:id="rId28"/>
+    <hyperlink ref="H46" r:id="rId29"/>
+    <hyperlink ref="H47" r:id="rId30"/>
+    <hyperlink ref="H49" r:id="rId31"/>
+    <hyperlink ref="H52" r:id="rId32"/>
+    <hyperlink ref="H53" r:id="rId33"/>
+    <hyperlink ref="H54" r:id="rId34"/>
+    <hyperlink ref="H12" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId30"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed pins for better board layout, updated sketch, cleaned up schematic, update BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
   <si>
     <t>RefDes</t>
   </si>
@@ -201,12 +201,6 @@
     <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/3-644456-8/A31118-ND/698350</t>
   </si>
   <si>
-    <t>https://www.sparkfun.com/products/11113</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/2378</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/infineon-technologies/IRF7416PBF/IRF7416PBF-ND/808018</t>
   </si>
   <si>
@@ -285,9 +279,6 @@
     <t>Sparkfun</t>
   </si>
   <si>
-    <t>Adafruit</t>
-  </si>
-  <si>
     <t>35HD</t>
   </si>
   <si>
@@ -300,33 +291,6 @@
     <t>Order Qty.</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/switchcraft-inc/35RAPC4BHN3/SC2405-ND/1288738</t>
-  </si>
-  <si>
-    <t>poss replacement for phone conn</t>
-  </si>
-  <si>
-    <t>http://www.switchcraft.com/Drawings/35rapc__hn3_cd.pdf</t>
-  </si>
-  <si>
-    <t>http://www.cui.com/product/resource/pd-40v.pdf</t>
-  </si>
-  <si>
-    <t>4-pin</t>
-  </si>
-  <si>
-    <t>1/4 jack</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/switchcraft-inc/297/SC1084-ND/109512</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/switchcraft-inc/RA49C14B/SC1541-ND/1289209</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Neutrik/NP3TT-P-R/?qs=sGAEpiMZZMvlX3nhDDO4ADUfAUIJI3vk17qNd8zaPfU%3d</t>
-  </si>
-  <si>
     <t>http://www.mouser.com/ProductDetail/Neutrik/NC3MXX-BAG/?qs=sGAEpiMZZMv0W4pxf2HiVxwZWAc2WDw0SRp5UVw1szU%3d</t>
   </si>
   <si>
@@ -336,20 +300,32 @@
     <t>http://www.mouser.com/ProductDetail/Neutrik/BXX-2-RED/?qs=%2fha2pyFaduh9bwlS2wJrYXf3Cx2jUt5OYrvSBPEHSYg%3d</t>
   </si>
   <si>
-    <t>Neutrik XLR</t>
-  </si>
-  <si>
     <t>640456-3</t>
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/640456-3/A19470-ND/259010</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sparkfun-electronics/DEV-11113/1568-1055-ND/5140820</t>
+  </si>
+  <si>
+    <t>XLR header base (red)</t>
+  </si>
+  <si>
+    <t>XLR 3-pin plug</t>
+  </si>
+  <si>
+    <t>3.5-8mm cable</t>
+  </si>
+  <si>
+    <t>XLR three-pin socket</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,13 +468,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -860,14 +829,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -884,10 +853,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1245,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,17 +1232,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="9"/>
+      <c r="A1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
@@ -1285,15 +1254,15 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
@@ -1401,7 +1370,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1450,19 +1419,21 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="2" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1515,111 +1486,117 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="2" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B17" s="6">
         <v>1</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B19" s="6">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B20" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
@@ -1628,93 +1605,89 @@
         <v>36</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B22" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="6">
-        <v>2</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="2" t="s">
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="B29" s="6">
         <v>1</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>89</v>
+      <c r="C29" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B30" s="6">
         <v>1</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>72</v>
-      </c>
+      <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
@@ -1725,7 +1698,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="6">
         <v>1</v>
@@ -1736,12 +1709,12 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B32" s="6">
         <v>1</v>
@@ -1752,28 +1725,23 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="6">
-        <v>1</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="2" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1784,9 +1752,11 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1795,134 +1765,99 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="6"/>
+        <v>97</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
       <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="D36" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
+      <c r="H36" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
+      <c r="H37" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
+      <c r="A38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="6">
+        <v>1</v>
+      </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" t="s">
-        <v>94</v>
+      <c r="H38" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="H39" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H42" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H43" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="H42" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H45" t="s">
-        <v>98</v>
-      </c>
+      <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H46" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H47" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H49" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H52" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="53" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H53" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="H54" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="8:19" x14ac:dyDescent="0.25">
-      <c r="L58" s="5" t="s">
+      <c r="H46" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="2"/>
+    </row>
+    <row r="57" spans="12:19" x14ac:dyDescent="0.25">
+      <c r="L57" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M58" s="6">
-        <v>1</v>
-      </c>
-      <c r="N58" s="6" t="s">
+      <c r="M57" s="6">
+        <v>1</v>
+      </c>
+      <c r="N57" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O58" s="6"/>
-      <c r="P58" s="6" t="s">
+      <c r="O57" s="6"/>
+      <c r="P57" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q58" s="6"/>
-      <c r="R58" s="6"/>
-      <c r="S58" s="2" t="s">
+      <c r="Q57" s="6"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="2" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="A25:B26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1"/>
@@ -1931,7 +1866,7 @@
     <hyperlink ref="H7" r:id="rId4"/>
     <hyperlink ref="H8" r:id="rId5"/>
     <hyperlink ref="H9" r:id="rId6"/>
-    <hyperlink ref="S58" r:id="rId7"/>
+    <hyperlink ref="S57" r:id="rId7"/>
     <hyperlink ref="H11" r:id="rId8"/>
     <hyperlink ref="H13" r:id="rId9"/>
     <hyperlink ref="H14" r:id="rId10"/>
@@ -1943,25 +1878,18 @@
     <hyperlink ref="H20" r:id="rId16"/>
     <hyperlink ref="H21" r:id="rId17"/>
     <hyperlink ref="H22" r:id="rId18"/>
-    <hyperlink ref="H23" r:id="rId19"/>
-    <hyperlink ref="H6" r:id="rId20"/>
+    <hyperlink ref="H6" r:id="rId19"/>
+    <hyperlink ref="H29" r:id="rId20"/>
     <hyperlink ref="H30" r:id="rId21"/>
     <hyperlink ref="H31" r:id="rId22"/>
     <hyperlink ref="H32" r:id="rId23"/>
-    <hyperlink ref="H33" r:id="rId24"/>
-    <hyperlink ref="H29" r:id="rId25"/>
-    <hyperlink ref="H39" r:id="rId26"/>
-    <hyperlink ref="H40" r:id="rId27"/>
-    <hyperlink ref="H43" r:id="rId28"/>
-    <hyperlink ref="H46" r:id="rId29"/>
-    <hyperlink ref="H47" r:id="rId30"/>
-    <hyperlink ref="H49" r:id="rId31"/>
-    <hyperlink ref="H52" r:id="rId32"/>
-    <hyperlink ref="H53" r:id="rId33"/>
-    <hyperlink ref="H54" r:id="rId34"/>
-    <hyperlink ref="H12" r:id="rId35"/>
+    <hyperlink ref="H28" r:id="rId24"/>
+    <hyperlink ref="H37" r:id="rId25"/>
+    <hyperlink ref="H38" r:id="rId26"/>
+    <hyperlink ref="H12" r:id="rId27"/>
+    <hyperlink ref="H36" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId36"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>